<commit_message>
statement for sales transaction Excel and PDF
</commit_message>
<xml_diff>
--- a/src/files/tempPDF/achatClient.xlsx
+++ b/src/files/tempPDF/achatClient.xlsx
@@ -11,23 +11,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
-  <si>
-    <t>Date de génération : 13/01/2025</t>
-  </si>
-  <si>
-    <t>Liste des comptes commerçants</t>
-  </si>
-  <si>
-    <t>Date exacte : 12/12/2024</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+  <si>
+    <t>Édité le : 16/01/2025</t>
+  </si>
+  <si>
+    <t>Liste des achats du commerçant : ali jemaa</t>
+  </si>
+  <si>
+    <t>le : 02/12/2024 à 16/01/2025</t>
   </si>
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Client</t>
-  </si>
-  <si>
     <t>Article</t>
   </si>
   <si>
@@ -46,9 +43,6 @@
     <t>2024-12-12</t>
   </si>
   <si>
-    <t>ali jemaa</t>
-  </si>
-  <si>
     <t>thon</t>
   </si>
   <si>
@@ -58,25 +52,34 @@
     <t>800,00</t>
   </si>
   <si>
-    <t>mohamed1 amich</t>
-  </si>
-  <si>
-    <t>Sardine</t>
+    <t>2024-12-13</t>
+  </si>
+  <si>
+    <t>Korradh</t>
+  </si>
+  <si>
+    <t>5,00</t>
+  </si>
+  <si>
+    <t>Morjen</t>
+  </si>
+  <si>
+    <t>24 000,00</t>
+  </si>
+  <si>
+    <t>2024-12-02</t>
+  </si>
+  <si>
+    <t>Balamit</t>
   </si>
   <si>
     <t>50,00</t>
   </si>
   <si>
-    <t>ferhat Jemaa</t>
-  </si>
-  <si>
-    <t>36 000,00</t>
-  </si>
-  <si>
-    <t>bogue</t>
-  </si>
-  <si>
-    <t>2,00</t>
+    <t>2025-01-03</t>
+  </si>
+  <si>
+    <t>10,00</t>
   </si>
   <si>
     <t>Total</t>
@@ -85,7 +88,7 @@
     <t/>
   </si>
   <si>
-    <t>36 872,00</t>
+    <t>24 885,00</t>
   </si>
 </sst>
 </file>
@@ -502,12 +505,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="3" width="20" customWidth="1"/>
-    <col min="4" max="7" width="15" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -521,7 +524,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" ht="40" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -532,7 +535,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" ht="70" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -543,7 +546,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -562,137 +565,139 @@
       <c r="F5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="5" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="6">
+        <v>10</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="6" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6">
+        <v>10</v>
+      </c>
+      <c r="D7" s="6">
+        <v>20</v>
+      </c>
+      <c r="E7" s="6">
+        <v>40</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="6">
-        <v>2</v>
-      </c>
-      <c r="F6" s="6">
-        <v>10</v>
-      </c>
-      <c r="G6" s="6" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="6">
-        <v>10</v>
-      </c>
-      <c r="E7" s="6">
-        <v>20</v>
-      </c>
-      <c r="F7" s="6">
-        <v>40</v>
-      </c>
-      <c r="G7" s="6" t="s">
+      <c r="B8" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="6">
+        <v>100</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6">
+        <v>5</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="6" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="6">
-        <v>2</v>
-      </c>
-      <c r="E8" s="6">
-        <v>10</v>
-      </c>
-      <c r="F8" s="6">
-        <v>5</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>16</v>
+      <c r="C9" s="6">
+        <v>50</v>
       </c>
       <c r="D9" s="6">
         <v>12</v>
       </c>
-      <c r="F9" s="6">
-        <v>3000</v>
-      </c>
-      <c r="G9" s="6" t="s">
+      <c r="E9" s="6">
+        <v>2000</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="C10" s="6">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6">
+        <v>5</v>
+      </c>
+      <c r="E10" s="6">
         <v>10</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="6">
-        <v>1</v>
-      </c>
-      <c r="F10" s="6">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="6">
         <v>2</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="E11" s="6">
+        <v>5</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="6" t="s">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="6">
-        <v>27</v>
-      </c>
-      <c r="E11" s="6">
-        <v>30</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="6" t="s">
+      <c r="B12" s="6" t="s">
         <v>24</v>
+      </c>
+      <c r="C12" s="6">
+        <v>165</v>
+      </c>
+      <c r="D12" s="6">
+        <v>38</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>